<commit_message>
Resolved Issue #4 aka DE1388
Resolved Issue #4 aka DE1388. CSV file exported was using 2 different
methodologies to organize header vs row data. Now uniformed
</commit_message>
<xml_diff>
--- a/samplefiles/providers/providers.xlsx
+++ b/samplefiles/providers/providers.xlsx
@@ -11,7 +11,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="79">
+  <si>
+    <t>PROVIDER_ID</t>
+  </si>
   <si>
     <t>PROVIDER_NAME</t>
   </si>
@@ -28,13 +31,223 @@
     <t>SCHEMA</t>
   </si>
   <si>
-    <t>TEST</t>
-  </si>
-  <si>
-    <t>postscndryunivsrvy2013dirinfo</t>
-  </si>
-  <si>
-    <t>XLSX</t>
+    <t>005</t>
+  </si>
+  <si>
+    <t>WIRELESS</t>
+  </si>
+  <si>
+    <t>GS00Q13NSA3000</t>
+  </si>
+  <si>
+    <t>david.larrimore@gmail.com</t>
+  </si>
+  <si>
+    <t>xlsx</t>
+  </si>
+  <si>
+    <t>GS00Q13NSA3001</t>
+  </si>
+  <si>
+    <t>GS00Q13NSA3002</t>
+  </si>
+  <si>
+    <t>GS00Q13NSA3003</t>
+  </si>
+  <si>
+    <t>003</t>
+  </si>
+  <si>
+    <t>OS3</t>
+  </si>
+  <si>
+    <t>GS02Q14DCR0001</t>
+  </si>
+  <si>
+    <t>GS02Q14DCR0002</t>
+  </si>
+  <si>
+    <t>GS02Q14DCR0004</t>
+  </si>
+  <si>
+    <t>GS02Q14DCR0006</t>
+  </si>
+  <si>
+    <t>GS02Q14DCR0007</t>
+  </si>
+  <si>
+    <t>GS02Q14DCR0008</t>
+  </si>
+  <si>
+    <t>GS02Q14DCR0009</t>
+  </si>
+  <si>
+    <t>GS02Q14DCR0011</t>
+  </si>
+  <si>
+    <t>GS02Q14DCR0012</t>
+  </si>
+  <si>
+    <t>GS02Q14DCR0015</t>
+  </si>
+  <si>
+    <t>004</t>
+  </si>
+  <si>
+    <t>PM</t>
+  </si>
+  <si>
+    <t>GS03FAA004</t>
+  </si>
+  <si>
+    <t>PM_FAII</t>
+  </si>
+  <si>
+    <t>GS03FAA005</t>
+  </si>
+  <si>
+    <t>GS03FAA006</t>
+  </si>
+  <si>
+    <t>GS03FPM001</t>
+  </si>
+  <si>
+    <t>GS03FPM003</t>
+  </si>
+  <si>
+    <t>GS03FPM004</t>
+  </si>
+  <si>
+    <t>GS03FPM005</t>
+  </si>
+  <si>
+    <t>GS03FPM006</t>
+  </si>
+  <si>
+    <t>GS03FPM007</t>
+  </si>
+  <si>
+    <t>GS03FPM008</t>
+  </si>
+  <si>
+    <t>GS03FPM009</t>
+  </si>
+  <si>
+    <t>GS03FPM010</t>
+  </si>
+  <si>
+    <t>GS03FPM011</t>
+  </si>
+  <si>
+    <t>002</t>
+  </si>
+  <si>
+    <t>JANSAN</t>
+  </si>
+  <si>
+    <t>GS07FBA385</t>
+  </si>
+  <si>
+    <t>GS07FBA386</t>
+  </si>
+  <si>
+    <t>GS07FBA387</t>
+  </si>
+  <si>
+    <t>GS07FBA388</t>
+  </si>
+  <si>
+    <t>GS07FBA389</t>
+  </si>
+  <si>
+    <t>GS07FBA390</t>
+  </si>
+  <si>
+    <t>GS07FBA391</t>
+  </si>
+  <si>
+    <t>GS07FBA392</t>
+  </si>
+  <si>
+    <t>GS07FBA393</t>
+  </si>
+  <si>
+    <t>GS07FBA394</t>
+  </si>
+  <si>
+    <t>GS07FBA395</t>
+  </si>
+  <si>
+    <t>GS07FBA396</t>
+  </si>
+  <si>
+    <t>GS07FBA397</t>
+  </si>
+  <si>
+    <t>GS07FBA398</t>
+  </si>
+  <si>
+    <t>GS07FBA399</t>
+  </si>
+  <si>
+    <t>GS07FBA400</t>
+  </si>
+  <si>
+    <t>GS07FBA401</t>
+  </si>
+  <si>
+    <t>GS07FBA407</t>
+  </si>
+  <si>
+    <t>001</t>
+  </si>
+  <si>
+    <t>MRO</t>
+  </si>
+  <si>
+    <t>GS23FBA005</t>
+  </si>
+  <si>
+    <t>GS23FBA006</t>
+  </si>
+  <si>
+    <t>GS23FBA007</t>
+  </si>
+  <si>
+    <t>GS23FBA008</t>
+  </si>
+  <si>
+    <t>GS23FBA009</t>
+  </si>
+  <si>
+    <t>GS23FBA012</t>
+  </si>
+  <si>
+    <t>GS23FBA013</t>
+  </si>
+  <si>
+    <t>GS23FBA014</t>
+  </si>
+  <si>
+    <t>GS23FBA015</t>
+  </si>
+  <si>
+    <t>GS23FBA016</t>
+  </si>
+  <si>
+    <t>GS23FBA017</t>
+  </si>
+  <si>
+    <t>006</t>
+  </si>
+  <si>
+    <t>DDS3</t>
+  </si>
+  <si>
+    <t>GS33FBA016</t>
+  </si>
+  <si>
+    <t>GS33FCA001</t>
   </si>
 </sst>
 </file>
@@ -56,14 +269,14 @@
       <name val="Helvetica"/>
     </font>
     <font>
-      <sz val="12"/>
+      <sz val="10"/>
       <color indexed="8"/>
-      <name val="Verdana"/>
+      <name val="Arial"/>
     </font>
     <font>
-      <sz val="15"/>
+      <sz val="13"/>
       <color indexed="8"/>
-      <name val="Verdana"/>
+      <name val="Arial"/>
     </font>
     <font>
       <sz val="0"/>
@@ -108,17 +321,14 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
+      <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="1" fontId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -1370,18 +1580,19 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:F59"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="16.75" style="1" customWidth="1"/>
-    <col min="2" max="2" width="24" style="1" customWidth="1"/>
-    <col min="3" max="3" width="19.75" style="1" customWidth="1"/>
-    <col min="4" max="4" width="17.25" style="1" customWidth="1"/>
+    <col min="1" max="1" width="10.875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="16.75" style="1" customWidth="1"/>
+    <col min="3" max="3" width="19.875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="19.75" style="1" customWidth="1"/>
     <col min="5" max="5" width="17.25" style="1" customWidth="1"/>
-    <col min="6" max="256" width="10.875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="17.25" style="1" customWidth="1"/>
+    <col min="7" max="256" width="10.875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="20" customHeight="1">
@@ -1400,19 +1611,1169 @@
       <c r="E1" t="s" s="2">
         <v>4</v>
       </c>
+      <c r="F1" t="s" s="2">
+        <v>5</v>
+      </c>
     </row>
     <row r="2" ht="20" customHeight="1">
       <c r="A2" t="s" s="2">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s" s="2">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s" s="2">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s" s="2">
+        <v>9</v>
+      </c>
+      <c r="E2" t="s" s="2">
+        <v>10</v>
+      </c>
+      <c r="F2" t="s" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" ht="20" customHeight="1">
+      <c r="A3" t="s" s="2">
         <v>6</v>
       </c>
-      <c r="C2" s="3"/>
-      <c r="D2" t="s" s="2">
+      <c r="B3" t="s" s="2">
         <v>7</v>
       </c>
-      <c r="E2" s="3"/>
+      <c r="C3" t="s" s="2">
+        <v>11</v>
+      </c>
+      <c r="D3" t="s" s="2">
+        <v>9</v>
+      </c>
+      <c r="E3" t="s" s="2">
+        <v>10</v>
+      </c>
+      <c r="F3" t="s" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" ht="20" customHeight="1">
+      <c r="A4" t="s" s="2">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s" s="2">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s" s="2">
+        <v>12</v>
+      </c>
+      <c r="D4" t="s" s="2">
+        <v>9</v>
+      </c>
+      <c r="E4" t="s" s="2">
+        <v>10</v>
+      </c>
+      <c r="F4" t="s" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" ht="20" customHeight="1">
+      <c r="A5" t="s" s="2">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s" s="2">
+        <v>7</v>
+      </c>
+      <c r="C5" t="s" s="2">
+        <v>13</v>
+      </c>
+      <c r="D5" t="s" s="2">
+        <v>9</v>
+      </c>
+      <c r="E5" t="s" s="2">
+        <v>10</v>
+      </c>
+      <c r="F5" t="s" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" ht="20" customHeight="1">
+      <c r="A6" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="B6" t="s" s="2">
+        <v>15</v>
+      </c>
+      <c r="C6" t="s" s="2">
+        <v>16</v>
+      </c>
+      <c r="D6" t="s" s="2">
+        <v>9</v>
+      </c>
+      <c r="E6" t="s" s="2">
+        <v>10</v>
+      </c>
+      <c r="F6" t="s" s="2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" ht="20" customHeight="1">
+      <c r="A7" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="B7" t="s" s="2">
+        <v>15</v>
+      </c>
+      <c r="C7" t="s" s="2">
+        <v>17</v>
+      </c>
+      <c r="D7" t="s" s="2">
+        <v>9</v>
+      </c>
+      <c r="E7" t="s" s="2">
+        <v>10</v>
+      </c>
+      <c r="F7" t="s" s="2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" ht="20" customHeight="1">
+      <c r="A8" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="B8" t="s" s="2">
+        <v>15</v>
+      </c>
+      <c r="C8" t="s" s="2">
+        <v>18</v>
+      </c>
+      <c r="D8" t="s" s="2">
+        <v>9</v>
+      </c>
+      <c r="E8" t="s" s="2">
+        <v>10</v>
+      </c>
+      <c r="F8" t="s" s="2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" ht="20" customHeight="1">
+      <c r="A9" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="B9" t="s" s="2">
+        <v>15</v>
+      </c>
+      <c r="C9" t="s" s="2">
+        <v>19</v>
+      </c>
+      <c r="D9" t="s" s="2">
+        <v>9</v>
+      </c>
+      <c r="E9" t="s" s="2">
+        <v>10</v>
+      </c>
+      <c r="F9" t="s" s="2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" ht="20" customHeight="1">
+      <c r="A10" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="B10" t="s" s="2">
+        <v>15</v>
+      </c>
+      <c r="C10" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="D10" t="s" s="2">
+        <v>9</v>
+      </c>
+      <c r="E10" t="s" s="2">
+        <v>10</v>
+      </c>
+      <c r="F10" t="s" s="2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" ht="20" customHeight="1">
+      <c r="A11" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="B11" t="s" s="2">
+        <v>15</v>
+      </c>
+      <c r="C11" t="s" s="2">
+        <v>21</v>
+      </c>
+      <c r="D11" t="s" s="2">
+        <v>9</v>
+      </c>
+      <c r="E11" t="s" s="2">
+        <v>10</v>
+      </c>
+      <c r="F11" t="s" s="2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" ht="20" customHeight="1">
+      <c r="A12" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="B12" t="s" s="2">
+        <v>15</v>
+      </c>
+      <c r="C12" t="s" s="2">
+        <v>22</v>
+      </c>
+      <c r="D12" t="s" s="2">
+        <v>9</v>
+      </c>
+      <c r="E12" t="s" s="2">
+        <v>10</v>
+      </c>
+      <c r="F12" t="s" s="2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" ht="20" customHeight="1">
+      <c r="A13" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="B13" t="s" s="2">
+        <v>15</v>
+      </c>
+      <c r="C13" t="s" s="2">
+        <v>23</v>
+      </c>
+      <c r="D13" t="s" s="2">
+        <v>9</v>
+      </c>
+      <c r="E13" t="s" s="2">
+        <v>10</v>
+      </c>
+      <c r="F13" t="s" s="2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" ht="20" customHeight="1">
+      <c r="A14" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="B14" t="s" s="2">
+        <v>15</v>
+      </c>
+      <c r="C14" t="s" s="2">
+        <v>24</v>
+      </c>
+      <c r="D14" t="s" s="2">
+        <v>9</v>
+      </c>
+      <c r="E14" t="s" s="2">
+        <v>10</v>
+      </c>
+      <c r="F14" t="s" s="2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" ht="20" customHeight="1">
+      <c r="A15" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s" s="2">
+        <v>15</v>
+      </c>
+      <c r="C15" t="s" s="2">
+        <v>25</v>
+      </c>
+      <c r="D15" t="s" s="2">
+        <v>9</v>
+      </c>
+      <c r="E15" t="s" s="2">
+        <v>10</v>
+      </c>
+      <c r="F15" t="s" s="2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" ht="20" customHeight="1">
+      <c r="A16" t="s" s="2">
+        <v>26</v>
+      </c>
+      <c r="B16" t="s" s="2">
+        <v>27</v>
+      </c>
+      <c r="C16" t="s" s="2">
+        <v>28</v>
+      </c>
+      <c r="D16" t="s" s="2">
+        <v>9</v>
+      </c>
+      <c r="E16" t="s" s="2">
+        <v>10</v>
+      </c>
+      <c r="F16" t="s" s="2">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="17" ht="20" customHeight="1">
+      <c r="A17" t="s" s="2">
+        <v>26</v>
+      </c>
+      <c r="B17" t="s" s="2">
+        <v>27</v>
+      </c>
+      <c r="C17" t="s" s="2">
+        <v>30</v>
+      </c>
+      <c r="D17" t="s" s="2">
+        <v>9</v>
+      </c>
+      <c r="E17" t="s" s="2">
+        <v>10</v>
+      </c>
+      <c r="F17" t="s" s="2">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18" ht="20" customHeight="1">
+      <c r="A18" t="s" s="2">
+        <v>26</v>
+      </c>
+      <c r="B18" t="s" s="2">
+        <v>27</v>
+      </c>
+      <c r="C18" t="s" s="2">
+        <v>31</v>
+      </c>
+      <c r="D18" t="s" s="2">
+        <v>9</v>
+      </c>
+      <c r="E18" t="s" s="2">
+        <v>10</v>
+      </c>
+      <c r="F18" t="s" s="2">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="19" ht="20" customHeight="1">
+      <c r="A19" t="s" s="2">
+        <v>26</v>
+      </c>
+      <c r="B19" t="s" s="2">
+        <v>27</v>
+      </c>
+      <c r="C19" t="s" s="2">
+        <v>32</v>
+      </c>
+      <c r="D19" t="s" s="2">
+        <v>9</v>
+      </c>
+      <c r="E19" t="s" s="2">
+        <v>10</v>
+      </c>
+      <c r="F19" t="s" s="2">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="20" ht="20" customHeight="1">
+      <c r="A20" t="s" s="2">
+        <v>26</v>
+      </c>
+      <c r="B20" t="s" s="2">
+        <v>27</v>
+      </c>
+      <c r="C20" t="s" s="2">
+        <v>33</v>
+      </c>
+      <c r="D20" t="s" s="2">
+        <v>9</v>
+      </c>
+      <c r="E20" t="s" s="2">
+        <v>10</v>
+      </c>
+      <c r="F20" t="s" s="2">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="21" ht="20" customHeight="1">
+      <c r="A21" t="s" s="2">
+        <v>26</v>
+      </c>
+      <c r="B21" t="s" s="2">
+        <v>27</v>
+      </c>
+      <c r="C21" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="D21" t="s" s="2">
+        <v>9</v>
+      </c>
+      <c r="E21" t="s" s="2">
+        <v>10</v>
+      </c>
+      <c r="F21" t="s" s="2">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="22" ht="20" customHeight="1">
+      <c r="A22" t="s" s="2">
+        <v>26</v>
+      </c>
+      <c r="B22" t="s" s="2">
+        <v>27</v>
+      </c>
+      <c r="C22" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="D22" t="s" s="2">
+        <v>9</v>
+      </c>
+      <c r="E22" t="s" s="2">
+        <v>10</v>
+      </c>
+      <c r="F22" t="s" s="2">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="23" ht="20" customHeight="1">
+      <c r="A23" t="s" s="2">
+        <v>26</v>
+      </c>
+      <c r="B23" t="s" s="2">
+        <v>27</v>
+      </c>
+      <c r="C23" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="D23" t="s" s="2">
+        <v>9</v>
+      </c>
+      <c r="E23" t="s" s="2">
+        <v>10</v>
+      </c>
+      <c r="F23" t="s" s="2">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="24" ht="20" customHeight="1">
+      <c r="A24" t="s" s="2">
+        <v>26</v>
+      </c>
+      <c r="B24" t="s" s="2">
+        <v>27</v>
+      </c>
+      <c r="C24" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="D24" t="s" s="2">
+        <v>9</v>
+      </c>
+      <c r="E24" t="s" s="2">
+        <v>10</v>
+      </c>
+      <c r="F24" t="s" s="2">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="25" ht="20" customHeight="1">
+      <c r="A25" t="s" s="2">
+        <v>26</v>
+      </c>
+      <c r="B25" t="s" s="2">
+        <v>27</v>
+      </c>
+      <c r="C25" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="D25" t="s" s="2">
+        <v>9</v>
+      </c>
+      <c r="E25" t="s" s="2">
+        <v>10</v>
+      </c>
+      <c r="F25" t="s" s="2">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="26" ht="20" customHeight="1">
+      <c r="A26" t="s" s="2">
+        <v>26</v>
+      </c>
+      <c r="B26" t="s" s="2">
+        <v>27</v>
+      </c>
+      <c r="C26" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="D26" t="s" s="2">
+        <v>9</v>
+      </c>
+      <c r="E26" t="s" s="2">
+        <v>10</v>
+      </c>
+      <c r="F26" t="s" s="2">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="27" ht="20" customHeight="1">
+      <c r="A27" t="s" s="2">
+        <v>26</v>
+      </c>
+      <c r="B27" t="s" s="2">
+        <v>27</v>
+      </c>
+      <c r="C27" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="D27" t="s" s="2">
+        <v>9</v>
+      </c>
+      <c r="E27" t="s" s="2">
+        <v>10</v>
+      </c>
+      <c r="F27" t="s" s="2">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="28" ht="20" customHeight="1">
+      <c r="A28" t="s" s="2">
+        <v>26</v>
+      </c>
+      <c r="B28" t="s" s="2">
+        <v>27</v>
+      </c>
+      <c r="C28" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="D28" t="s" s="2">
+        <v>9</v>
+      </c>
+      <c r="E28" t="s" s="2">
+        <v>10</v>
+      </c>
+      <c r="F28" t="s" s="2">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="29" ht="20" customHeight="1">
+      <c r="A29" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="B29" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="C29" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="D29" t="s" s="2">
+        <v>9</v>
+      </c>
+      <c r="E29" t="s" s="2">
+        <v>10</v>
+      </c>
+      <c r="F29" t="s" s="2">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="30" ht="20" customHeight="1">
+      <c r="A30" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="B30" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="C30" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="D30" t="s" s="2">
+        <v>9</v>
+      </c>
+      <c r="E30" t="s" s="2">
+        <v>10</v>
+      </c>
+      <c r="F30" t="s" s="2">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="31" ht="20" customHeight="1">
+      <c r="A31" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="B31" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="C31" t="s" s="2">
+        <v>46</v>
+      </c>
+      <c r="D31" t="s" s="2">
+        <v>9</v>
+      </c>
+      <c r="E31" t="s" s="2">
+        <v>10</v>
+      </c>
+      <c r="F31" t="s" s="2">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="32" ht="20" customHeight="1">
+      <c r="A32" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="B32" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="C32" t="s" s="2">
+        <v>47</v>
+      </c>
+      <c r="D32" t="s" s="2">
+        <v>9</v>
+      </c>
+      <c r="E32" t="s" s="2">
+        <v>10</v>
+      </c>
+      <c r="F32" t="s" s="2">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="33" ht="20" customHeight="1">
+      <c r="A33" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="B33" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="C33" t="s" s="2">
+        <v>48</v>
+      </c>
+      <c r="D33" t="s" s="2">
+        <v>9</v>
+      </c>
+      <c r="E33" t="s" s="2">
+        <v>10</v>
+      </c>
+      <c r="F33" t="s" s="2">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="34" ht="20" customHeight="1">
+      <c r="A34" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="B34" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="C34" t="s" s="2">
+        <v>49</v>
+      </c>
+      <c r="D34" t="s" s="2">
+        <v>9</v>
+      </c>
+      <c r="E34" t="s" s="2">
+        <v>10</v>
+      </c>
+      <c r="F34" t="s" s="2">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="35" ht="20" customHeight="1">
+      <c r="A35" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="B35" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="C35" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="D35" t="s" s="2">
+        <v>9</v>
+      </c>
+      <c r="E35" t="s" s="2">
+        <v>10</v>
+      </c>
+      <c r="F35" t="s" s="2">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="36" ht="20" customHeight="1">
+      <c r="A36" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="B36" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="C36" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="D36" t="s" s="2">
+        <v>9</v>
+      </c>
+      <c r="E36" t="s" s="2">
+        <v>10</v>
+      </c>
+      <c r="F36" t="s" s="2">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="37" ht="20" customHeight="1">
+      <c r="A37" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="B37" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="C37" t="s" s="2">
+        <v>52</v>
+      </c>
+      <c r="D37" t="s" s="2">
+        <v>9</v>
+      </c>
+      <c r="E37" t="s" s="2">
+        <v>10</v>
+      </c>
+      <c r="F37" t="s" s="2">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="38" ht="20" customHeight="1">
+      <c r="A38" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="B38" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="C38" t="s" s="2">
+        <v>53</v>
+      </c>
+      <c r="D38" t="s" s="2">
+        <v>9</v>
+      </c>
+      <c r="E38" t="s" s="2">
+        <v>10</v>
+      </c>
+      <c r="F38" t="s" s="2">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="39" ht="20" customHeight="1">
+      <c r="A39" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="B39" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="C39" t="s" s="2">
+        <v>54</v>
+      </c>
+      <c r="D39" t="s" s="2">
+        <v>9</v>
+      </c>
+      <c r="E39" t="s" s="2">
+        <v>10</v>
+      </c>
+      <c r="F39" t="s" s="2">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="40" ht="20" customHeight="1">
+      <c r="A40" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="B40" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="C40" t="s" s="2">
+        <v>55</v>
+      </c>
+      <c r="D40" t="s" s="2">
+        <v>9</v>
+      </c>
+      <c r="E40" t="s" s="2">
+        <v>10</v>
+      </c>
+      <c r="F40" t="s" s="2">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="41" ht="20" customHeight="1">
+      <c r="A41" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="B41" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="C41" t="s" s="2">
+        <v>56</v>
+      </c>
+      <c r="D41" t="s" s="2">
+        <v>9</v>
+      </c>
+      <c r="E41" t="s" s="2">
+        <v>10</v>
+      </c>
+      <c r="F41" t="s" s="2">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="42" ht="20" customHeight="1">
+      <c r="A42" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="B42" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="C42" t="s" s="2">
+        <v>57</v>
+      </c>
+      <c r="D42" t="s" s="2">
+        <v>9</v>
+      </c>
+      <c r="E42" t="s" s="2">
+        <v>10</v>
+      </c>
+      <c r="F42" t="s" s="2">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="43" ht="20" customHeight="1">
+      <c r="A43" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="B43" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="C43" t="s" s="2">
+        <v>58</v>
+      </c>
+      <c r="D43" t="s" s="2">
+        <v>9</v>
+      </c>
+      <c r="E43" t="s" s="2">
+        <v>10</v>
+      </c>
+      <c r="F43" t="s" s="2">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="44" ht="20" customHeight="1">
+      <c r="A44" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="B44" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="C44" t="s" s="2">
+        <v>59</v>
+      </c>
+      <c r="D44" t="s" s="2">
+        <v>9</v>
+      </c>
+      <c r="E44" t="s" s="2">
+        <v>10</v>
+      </c>
+      <c r="F44" t="s" s="2">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="45" ht="20" customHeight="1">
+      <c r="A45" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="B45" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="C45" t="s" s="2">
+        <v>60</v>
+      </c>
+      <c r="D45" t="s" s="2">
+        <v>9</v>
+      </c>
+      <c r="E45" t="s" s="2">
+        <v>10</v>
+      </c>
+      <c r="F45" t="s" s="2">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="46" ht="20" customHeight="1">
+      <c r="A46" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="B46" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="C46" t="s" s="2">
+        <v>61</v>
+      </c>
+      <c r="D46" t="s" s="2">
+        <v>9</v>
+      </c>
+      <c r="E46" t="s" s="2">
+        <v>10</v>
+      </c>
+      <c r="F46" t="s" s="2">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="47" ht="20" customHeight="1">
+      <c r="A47" t="s" s="2">
+        <v>62</v>
+      </c>
+      <c r="B47" t="s" s="2">
+        <v>63</v>
+      </c>
+      <c r="C47" t="s" s="2">
+        <v>64</v>
+      </c>
+      <c r="D47" t="s" s="2">
+        <v>9</v>
+      </c>
+      <c r="E47" t="s" s="2">
+        <v>10</v>
+      </c>
+      <c r="F47" t="s" s="2">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="48" ht="20" customHeight="1">
+      <c r="A48" t="s" s="2">
+        <v>62</v>
+      </c>
+      <c r="B48" t="s" s="2">
+        <v>63</v>
+      </c>
+      <c r="C48" t="s" s="2">
+        <v>65</v>
+      </c>
+      <c r="D48" t="s" s="2">
+        <v>9</v>
+      </c>
+      <c r="E48" t="s" s="2">
+        <v>10</v>
+      </c>
+      <c r="F48" t="s" s="2">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="49" ht="20" customHeight="1">
+      <c r="A49" t="s" s="2">
+        <v>62</v>
+      </c>
+      <c r="B49" t="s" s="2">
+        <v>63</v>
+      </c>
+      <c r="C49" t="s" s="2">
+        <v>66</v>
+      </c>
+      <c r="D49" t="s" s="2">
+        <v>9</v>
+      </c>
+      <c r="E49" t="s" s="2">
+        <v>10</v>
+      </c>
+      <c r="F49" t="s" s="2">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="50" ht="20" customHeight="1">
+      <c r="A50" t="s" s="2">
+        <v>62</v>
+      </c>
+      <c r="B50" t="s" s="2">
+        <v>63</v>
+      </c>
+      <c r="C50" t="s" s="2">
+        <v>67</v>
+      </c>
+      <c r="D50" t="s" s="2">
+        <v>9</v>
+      </c>
+      <c r="E50" t="s" s="2">
+        <v>10</v>
+      </c>
+      <c r="F50" t="s" s="2">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="51" ht="20" customHeight="1">
+      <c r="A51" t="s" s="2">
+        <v>62</v>
+      </c>
+      <c r="B51" t="s" s="2">
+        <v>63</v>
+      </c>
+      <c r="C51" t="s" s="2">
+        <v>68</v>
+      </c>
+      <c r="D51" t="s" s="2">
+        <v>9</v>
+      </c>
+      <c r="E51" t="s" s="2">
+        <v>10</v>
+      </c>
+      <c r="F51" t="s" s="2">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="52" ht="20" customHeight="1">
+      <c r="A52" t="s" s="2">
+        <v>62</v>
+      </c>
+      <c r="B52" t="s" s="2">
+        <v>63</v>
+      </c>
+      <c r="C52" t="s" s="2">
+        <v>69</v>
+      </c>
+      <c r="D52" t="s" s="2">
+        <v>9</v>
+      </c>
+      <c r="E52" t="s" s="2">
+        <v>10</v>
+      </c>
+      <c r="F52" t="s" s="2">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="53" ht="20" customHeight="1">
+      <c r="A53" t="s" s="2">
+        <v>62</v>
+      </c>
+      <c r="B53" t="s" s="2">
+        <v>63</v>
+      </c>
+      <c r="C53" t="s" s="2">
+        <v>70</v>
+      </c>
+      <c r="D53" t="s" s="2">
+        <v>9</v>
+      </c>
+      <c r="E53" t="s" s="2">
+        <v>10</v>
+      </c>
+      <c r="F53" t="s" s="2">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="54" ht="20" customHeight="1">
+      <c r="A54" t="s" s="2">
+        <v>62</v>
+      </c>
+      <c r="B54" t="s" s="2">
+        <v>63</v>
+      </c>
+      <c r="C54" t="s" s="2">
+        <v>71</v>
+      </c>
+      <c r="D54" t="s" s="2">
+        <v>9</v>
+      </c>
+      <c r="E54" t="s" s="2">
+        <v>10</v>
+      </c>
+      <c r="F54" t="s" s="2">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="55" ht="20" customHeight="1">
+      <c r="A55" t="s" s="2">
+        <v>62</v>
+      </c>
+      <c r="B55" t="s" s="2">
+        <v>63</v>
+      </c>
+      <c r="C55" t="s" s="2">
+        <v>72</v>
+      </c>
+      <c r="D55" t="s" s="2">
+        <v>9</v>
+      </c>
+      <c r="E55" t="s" s="2">
+        <v>10</v>
+      </c>
+      <c r="F55" t="s" s="2">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="56" ht="20" customHeight="1">
+      <c r="A56" t="s" s="2">
+        <v>62</v>
+      </c>
+      <c r="B56" t="s" s="2">
+        <v>63</v>
+      </c>
+      <c r="C56" t="s" s="2">
+        <v>73</v>
+      </c>
+      <c r="D56" t="s" s="2">
+        <v>9</v>
+      </c>
+      <c r="E56" t="s" s="2">
+        <v>10</v>
+      </c>
+      <c r="F56" t="s" s="2">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="57" ht="20" customHeight="1">
+      <c r="A57" t="s" s="2">
+        <v>62</v>
+      </c>
+      <c r="B57" t="s" s="2">
+        <v>63</v>
+      </c>
+      <c r="C57" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="D57" t="s" s="2">
+        <v>9</v>
+      </c>
+      <c r="E57" t="s" s="2">
+        <v>10</v>
+      </c>
+      <c r="F57" t="s" s="2">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="58" ht="20" customHeight="1">
+      <c r="A58" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="B58" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="C58" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="D58" t="s" s="2">
+        <v>9</v>
+      </c>
+      <c r="E58" t="s" s="2">
+        <v>10</v>
+      </c>
+      <c r="F58" t="s" s="2">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="59" ht="20" customHeight="1">
+      <c r="A59" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="B59" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="C59" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="D59" t="s" s="2">
+        <v>9</v>
+      </c>
+      <c r="E59" t="s" s="2">
+        <v>10</v>
+      </c>
+      <c r="F59" t="s" s="2">
+        <v>76</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>